<commit_message>
added dynmic test data
</commit_message>
<xml_diff>
--- a/testData/prod/productTemplate.xlsx
+++ b/testData/prod/productTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bharath\git\playwright-dady\testData\prod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EE11A4-877B-40AF-8272-4434424C11AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9460D67-6E59-416F-893C-4D8C3D6F8613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{4FC7762B-8720-454C-9CA6-94203251A910}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{4FC7762B-8720-454C-9CA6-94203251A910}"/>
   </bookViews>
   <sheets>
     <sheet name="productDetails" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="120">
   <si>
     <t>Package Attribute</t>
   </si>
@@ -85,9 +85,6 @@
     <t>3 Ply Box</t>
   </si>
   <si>
-    <t>Corrugated Box</t>
-  </si>
-  <si>
     <t>Packaging</t>
   </si>
   <si>
@@ -380,6 +377,27 @@
   </si>
   <si>
     <t>SurfaceareaSQM</t>
+  </si>
+  <si>
+    <t>CB-3BN4</t>
+  </si>
+  <si>
+    <t>4 Ply Box</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>4 ply box for packing cloths</t>
+  </si>
+  <si>
+    <t>0.550 kg</t>
+  </si>
+  <si>
+    <t>BUNDLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plastic Film </t>
   </si>
 </sst>
 </file>
@@ -900,8 +918,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{657772C1-EBF0-4C37-A613-849D5347B8D0}">
   <dimension ref="A1:BD20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +945,7 @@
   <sheetData>
     <row r="1" spans="1:56" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -935,7 +953,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
       <c r="G1" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" s="19"/>
       <c r="I1" s="19"/>
@@ -949,7 +967,7 @@
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
       <c r="S1" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T1" s="20"/>
       <c r="U1" s="20"/>
@@ -967,23 +985,23 @@
       <c r="AE1" s="19"/>
       <c r="AF1" s="19"/>
       <c r="AG1" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AH1" s="20"/>
       <c r="AI1" s="20"/>
       <c r="AJ1" s="20"/>
       <c r="AK1" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AL1" s="19"/>
       <c r="AM1" s="19"/>
       <c r="AN1" s="19"/>
       <c r="AO1" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AP1" s="20"/>
       <c r="AQ1" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AR1" s="19"/>
       <c r="AS1" s="19"/>
@@ -1001,7 +1019,7 @@
     </row>
     <row r="2" spans="1:56" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1010,163 +1028,163 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="AE2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="AK2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AL2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="AP2" s="3" t="s">
+      <c r="AQ2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="AQ2" s="1" t="s">
+      <c r="AR2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="BC2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:56" ht="43.5" x14ac:dyDescent="0.25">
@@ -1196,22 +1214,22 @@
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="7" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M3" s="7">
         <v>50</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="P3" s="7">
         <v>123455666</v>
@@ -1220,16 +1238,16 @@
         <v>123455666</v>
       </c>
       <c r="R3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>21</v>
       </c>
       <c r="V3" s="10" t="s">
         <v>12</v>
@@ -1247,22 +1265,22 @@
         <v>12</v>
       </c>
       <c r="AA3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB3" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="AB3" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="AC3" s="10">
         <v>1200</v>
       </c>
       <c r="AD3" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AE3" s="11">
         <v>44938</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG3" s="10">
         <v>4819100040</v>
@@ -1271,19 +1289,19 @@
         <v>48191010</v>
       </c>
       <c r="AI3" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ3" s="10" t="s">
         <v>26</v>
-      </c>
-      <c r="AJ3" s="10" t="s">
-        <v>27</v>
       </c>
       <c r="AK3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="AL3" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AM3" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN3" s="13">
         <v>0.32</v>
@@ -1319,22 +1337,190 @@
         <v>1828.57</v>
       </c>
       <c r="AY3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="AZ3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BA3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BB3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BC3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="BD3" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" s="7">
+        <v>60</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="P4" s="7">
+        <v>123455666</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>123455666</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="V4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC4" s="10">
+        <v>1300</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE4" s="11">
+        <v>44938</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="AG4" s="10">
+        <v>5819100040</v>
+      </c>
+      <c r="AH4" s="10">
+        <v>58191010</v>
+      </c>
+      <c r="AI4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM4" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN4" s="13">
+        <v>0.42</v>
+      </c>
+      <c r="AO4" s="6">
+        <v>400</v>
+      </c>
+      <c r="AP4" s="6">
+        <v>30</v>
+      </c>
+      <c r="AQ4" s="14">
+        <v>20</v>
+      </c>
+      <c r="AR4" s="14">
+        <v>32</v>
+      </c>
+      <c r="AS4" s="14">
+        <v>16</v>
+      </c>
+      <c r="AT4" s="14">
+        <v>32</v>
+      </c>
+      <c r="AU4" s="12">
+        <v>0.32</v>
+      </c>
+      <c r="AV4" s="12">
+        <v>0.64</v>
+      </c>
+      <c r="AW4" s="12">
+        <v>914.29</v>
+      </c>
+      <c r="AX4" s="12">
+        <v>1828.57</v>
+      </c>
+      <c r="AY4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="AZ4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BA4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BC4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="BD4" s="12" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1395,73 +1581,73 @@
     </row>
     <row r="2" spans="1:24" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="H2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="L2" s="15" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N2" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="O2" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="P2" s="16" t="s">
         <v>4</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>4</v>
@@ -1469,7 +1655,7 @@
     </row>
     <row r="3" spans="1:24" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="10">
         <v>14</v>
@@ -1493,7 +1679,7 @@
         <v>0.01</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="10">
         <v>10</v>
@@ -1505,7 +1691,7 @@
         <v>0.1</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N3" s="10">
         <v>10</v>
@@ -1543,13 +1729,13 @@
   <sheetData>
     <row r="1" spans="1:21" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
       <c r="E1" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
@@ -1557,7 +1743,7 @@
       <c r="I1" s="22"/>
       <c r="J1" s="22"/>
       <c r="K1" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L1" s="19"/>
       <c r="M1" s="19"/>
@@ -1575,34 +1761,34 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
@@ -1611,13 +1797,13 @@
         <v>5</v>
       </c>
       <c r="N2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>6</v>
@@ -1643,17 +1829,17 @@
         <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>11</v>
@@ -1684,7 +1870,7 @@
       </c>
       <c r="Q3" s="12"/>
       <c r="R3" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S3" s="10">
         <v>12</v>

</xml_diff>